<commit_message>
AddData 원복 & Tables 추가
</commit_message>
<xml_diff>
--- a/CSVToScriptableObject/Assets/Tables/TestTableFirst.xlsx
+++ b/CSVToScriptableObject/Assets/Tables/TestTableFirst.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Unity Project\CSVToScriptableObject\Assets\Tables\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Git Hub\CSVToScriptableObject\CSVToScriptableObject\Assets\Tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19D79927-7B93-4E99-B0CE-E872C1F76335}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7C54E09-FC6D-4813-B727-293ADD6BA7C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6585" yWindow="1875" windowWidth="28800" windowHeight="18255" xr2:uid="{950BFA12-91E0-4A26-A448-4D1BDCD4031A}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="28770" windowHeight="15450" xr2:uid="{950BFA12-91E0-4A26-A448-4D1BDCD4031A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -86,27 +86,27 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>name3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>name4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>desc3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>desc4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>name2</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>name3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>name4</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>desc2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>desc3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>desc4</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -503,10 +503,13 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="5" max="5" width="10.875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
@@ -555,10 +558,10 @@
         <v>1002</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D4" t="s">
         <v>9</v>
@@ -569,10 +572,10 @@
         <v>1003</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D5" t="s">
         <v>10</v>
@@ -583,10 +586,10 @@
         <v>1004</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D6" t="s">
         <v>11</v>

</xml_diff>